<commit_message>
Acquis, zone morte, pid
</commit_message>
<xml_diff>
--- a/PinSTM.xlsx
+++ b/PinSTM.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>PE7</t>
   </si>
@@ -353,6 +352,21 @@
   </si>
   <si>
     <t>LineInterrupt4</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>uaart</t>
+  </si>
+  <si>
+    <t>uart</t>
+  </si>
+  <si>
+    <t>détection antenne</t>
   </si>
 </sst>
 </file>
@@ -670,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +753,9 @@
       <c r="A8" t="s">
         <v>89</v>
       </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -826,190 +843,198 @@
         <v>77</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>98</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -1017,7 +1042,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
@@ -1025,33 +1050,33 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>68</v>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
         <v>75</v>
@@ -1059,7 +1084,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
         <v>75</v>
@@ -1067,7 +1092,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>75</v>
@@ -1075,7 +1100,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>75</v>
@@ -1083,65 +1108,73 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>7</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>